<commit_message>
add pseudo r-squared to tables; slight modifications to code
</commit_message>
<xml_diff>
--- a/Results_May_15_mostrecentupdateNovember18/combined_r_Only_Models_With_Surrogate_Current_Thesis.xlsx
+++ b/Results_May_15_mostrecentupdateNovember18/combined_r_Only_Models_With_Surrogate_Current_Thesis.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>K</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Model Name</t>
   </si>
   <si>
-    <t>K*</t>
-  </si>
-  <si>
     <t>Delta AICc</t>
   </si>
   <si>
@@ -72,6 +69,41 @@
   </si>
   <si>
     <t>Log-likelihood</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -81,7 +113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +269,30 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -431,7 +487,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -566,17 +622,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -622,7 +667,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -631,9 +676,10 @@
     <xf numFmtId="2" fontId="18" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="18" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1183,35 +1229,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1230,8 +1279,11 @@
       <c r="F2" s="6">
         <v>-527.99479874596</v>
       </c>
+      <c r="G2" s="4">
+        <v>0.64900000000000002</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1250,8 +1302,11 @@
       <c r="F3" s="6">
         <v>-532.52133986726403</v>
       </c>
+      <c r="G3" s="4">
+        <v>0.60099999999999998</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1270,8 +1325,11 @@
       <c r="F4" s="6">
         <v>-542.29259515181195</v>
       </c>
+      <c r="G4" s="4">
+        <v>0.48699999999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1290,8 +1348,11 @@
       <c r="F5" s="6">
         <v>-527.51758612692402</v>
       </c>
+      <c r="G5" s="4">
+        <v>0.65400000000000003</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1310,8 +1371,11 @@
       <c r="F6" s="6">
         <v>-542.22435878589704</v>
       </c>
+      <c r="G6" s="4">
+        <v>0.48799999999999999</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1329,6 +1393,9 @@
       </c>
       <c r="F7" s="7">
         <v>-550.30354497209203</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0.38300000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>